<commit_message>
Add preprocessed datasets without smote
</commit_message>
<xml_diff>
--- a/Preprocessed Data/lancet dataset/test_abc_lancet.xlsx
+++ b/Preprocessed Data/lancet dataset/test_abc_lancet.xlsx
@@ -474,7 +474,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-1.864812769550304</v>
+        <v>-1.416666666666667</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -486,13 +486,13 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>-0.5662668750180835</v>
+        <v>-0.5097753669697229</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.7371358013128344</v>
+        <v>0.75</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -510,10 +510,10 @@
         <v>1</v>
       </c>
       <c r="N2">
-        <v>0.2944232556588939</v>
+        <v>0.2197802197802198</v>
       </c>
       <c r="O2">
-        <v>0.4867773784927804</v>
+        <v>0.4203719417309194</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -524,7 +524,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.6626108794623501</v>
+        <v>-0.4166666666666667</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -536,13 +536,13 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>-0.009922273022458123</v>
+        <v>-0.01558650596374595</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>1.001144944885941</v>
+        <v>1.035714285714286</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -560,10 +560,10 @@
         <v>1</v>
       </c>
       <c r="N3">
-        <v>0.5444232556588938</v>
+        <v>0.4835164835164835</v>
       </c>
       <c r="O3">
-        <v>0.06441167956513537</v>
+        <v>0.01236372571126327</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -574,7 +574,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.7399579923069298</v>
+        <v>0.75</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -586,13 +586,13 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>-0.3871073518538086</v>
+        <v>-0.3506318426624211</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
-        <v>-0.3519019159262309</v>
+        <v>-0.4285714285714285</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -610,10 +610,10 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <v>-0.9555767443411062</v>
+        <v>-1.098901098901099</v>
       </c>
       <c r="O4">
-        <v>-0.3829325303479286</v>
+        <v>-0.4197739064325323</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -624,7 +624,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.44124242819157</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -636,13 +636,13 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.2721679477077184</v>
+        <v>0.2349881277857637</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>-0.8469190601258061</v>
+        <v>-0.9642857142857143</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -660,10 +660,10 @@
         <v>1</v>
       </c>
       <c r="N5">
-        <v>-0.1222434110077728</v>
+        <v>-0.2197802197802198</v>
       </c>
       <c r="O5">
-        <v>-0.3612703647568711</v>
+        <v>-0.3988481031289743</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -674,7 +674,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1.040508464828918</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -686,13 +686,13 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>-0.2685049753584531</v>
+        <v>-0.2452799202341297</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>-0.9459224889657211</v>
+        <v>-1.071428571428571</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -710,10 +710,10 @@
         <v>1</v>
       </c>
       <c r="N6">
-        <v>0.1694232556588939</v>
+        <v>0.08791208791208792</v>
       </c>
       <c r="O6">
-        <v>-0.7939169227049881</v>
+        <v>-0.8167877007895694</v>
       </c>
       <c r="P6">
         <v>1</v>
@@ -724,7 +724,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.4394075197849412</v>
+        <v>0.5</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -736,13 +736,13 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>-0.6054460723417193</v>
+        <v>-0.5445773994349328</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>-0.5169076306594226</v>
+        <v>-0.6071428571428571</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -760,10 +760,10 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <v>-0.4139100776744395</v>
+        <v>-0.5274725274725275</v>
       </c>
       <c r="O7">
-        <v>1.12358786260141</v>
+        <v>1.035535318452677</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -774,7 +774,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.4394075197849412</v>
+        <v>0.5</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -786,13 +786,13 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1.102766930968793</v>
+        <v>0.972791216048208</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0.3741232288998126</v>
+        <v>0.3571428571428572</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -810,10 +810,10 @@
         <v>1</v>
       </c>
       <c r="N8">
-        <v>-0.7055767443411062</v>
+        <v>-0.8351648351648352</v>
       </c>
       <c r="O8">
-        <v>0.9157890066493389</v>
+        <v>0.8348001718174527</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -824,7 +824,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.8401414831475926</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -836,13 +836,13 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>0.1076153189484482</v>
+        <v>0.08881959143188262</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>-1.506941919058573</v>
+        <v>-1.678571428571429</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -860,10 +860,10 @@
         <v>1</v>
       </c>
       <c r="N9">
-        <v>1.294423255658894</v>
+        <v>1.274725274725275</v>
       </c>
       <c r="O9">
-        <v>-2.670529001717799</v>
+        <v>-2.629608080055551</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -874,7 +874,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.641609409872895</v>
+        <v>1.5</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -886,13 +886,13 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>-0.5662668750180835</v>
+        <v>-0.5097753669697229</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0.1431152282733442</v>
+        <v>0.1071428571428571</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -910,10 +910,10 @@
         <v>1</v>
       </c>
       <c r="N10">
-        <v>-1.747243411007773</v>
+        <v>-1.934065934065934</v>
       </c>
       <c r="O10">
-        <v>0.889837767455833</v>
+        <v>0.8097310934483412</v>
       </c>
       <c r="P10">
         <v>1</v>
@@ -924,7 +924,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.4394075197849412</v>
+        <v>0.5</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -936,13 +936,13 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>-0.9188796509308039</v>
+        <v>-0.8229936591566098</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0.1431152282733442</v>
+        <v>0.1071428571428571</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -960,10 +960,10 @@
         <v>1</v>
       </c>
       <c r="N11">
-        <v>-0.4555767443411061</v>
+        <v>-0.5714285714285714</v>
       </c>
       <c r="O11">
-        <v>-0.02948488097408481</v>
+        <v>-0.07834100777740907</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -974,7 +974,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.1388570472629527</v>
+        <v>0.25</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -986,13 +986,13 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>0.6561240814793466</v>
+        <v>0.5760480459448177</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>-1.077927060752274</v>
+        <v>-1.214285714285714</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1010,10 +1010,10 @@
         <v>2</v>
       </c>
       <c r="N12">
-        <v>0.5860899223255606</v>
+        <v>0.5274725274725275</v>
       </c>
       <c r="O12">
-        <v>-0.3385489092396301</v>
+        <v>-0.3768990183559998</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1024,7 +1024,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.9403249739882554</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1036,13 +1036,13 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>-0.2721043188091638</v>
+        <v>-0.2484771390691747</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>-0.1208939152997625</v>
+        <v>-0.1785714285714286</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1060,10 +1060,10 @@
         <v>2</v>
       </c>
       <c r="N13">
-        <v>-0.8305767443411062</v>
+        <v>-0.967032967032967</v>
       </c>
       <c r="O13">
-        <v>0.0723047262643651</v>
+        <v>0.01998846396744502</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -1074,7 +1074,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.8401414831475926</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1086,13 +1086,13 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>-0.3299026665782132</v>
+        <v>-0.2998181596336889</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0.3411220859531743</v>
+        <v>0.3214285714285715</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1110,10 +1110,10 @@
         <v>1</v>
       </c>
       <c r="N14">
-        <v>-0.5389100776744394</v>
+        <v>-0.6593406593406593</v>
       </c>
       <c r="O14">
-        <v>-0.3000557313526077</v>
+        <v>-0.3397143395847679</v>
       </c>
       <c r="P14">
         <v>1</v>
@@ -1124,7 +1124,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-1.163528333665664</v>
+        <v>-0.8333333333333334</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1136,13 +1136,13 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>-0.6681327880595362</v>
+        <v>-0.6002606513792682</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>-0.8799202030724443</v>
+        <v>-1</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1160,10 +1160,10 @@
         <v>1</v>
       </c>
       <c r="N15">
-        <v>-0.08057674434110614</v>
+        <v>-0.1758241758241758</v>
       </c>
       <c r="O15">
-        <v>0.09211408096645847</v>
+        <v>0.03912443900761108</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -1174,7 +1174,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-0.4622438977810244</v>
+        <v>-0.25</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1186,13 +1186,13 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0.3357149670014565</v>
+        <v>0.291435568764699</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0.3411220859531743</v>
+        <v>0.3214285714285715</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1210,10 +1210,10 @@
         <v>1</v>
       </c>
       <c r="N16">
-        <v>-0.1222434110077728</v>
+        <v>-0.2197802197802198</v>
       </c>
       <c r="O16">
-        <v>0.04892319284550058</v>
+        <v>-0.002598260670128217</v>
       </c>
       <c r="P16">
         <v>1</v>
@@ -1224,7 +1224,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.1388570472629527</v>
+        <v>0.25</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1236,13 +1236,13 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>1.557245619922966</v>
+        <v>1.37649479264464</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17">
-        <v>0.3081209430065359</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1260,10 +1260,10 @@
         <v>2</v>
       </c>
       <c r="N17">
-        <v>1.544423255658894</v>
+        <v>1.538461538461539</v>
       </c>
       <c r="O17">
-        <v>-0.06825556449135912</v>
+        <v>-0.1157937589262557</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -1274,7 +1274,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-0.9631613519843386</v>
+        <v>-0.6666666666666666</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1286,13 +1286,13 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>-0.213654099105363</v>
+        <v>-0.196557074782836</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>-0.08789277235312419</v>
+        <v>-0.1428571428571428</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1310,10 +1310,10 @@
         <v>1</v>
       </c>
       <c r="N18">
-        <v>0.002756588992227194</v>
+        <v>-0.08791208791208792</v>
       </c>
       <c r="O18">
-        <v>0.2319814315553449</v>
+        <v>0.174237276858924</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -1324,7 +1324,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-1.063344842825001</v>
+        <v>-0.75</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1336,13 +1336,13 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>-0.1979824201759091</v>
+        <v>-0.1826362617967524</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>-0.05489162940648584</v>
+        <v>-0.1071428571428571</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1360,10 +1360,10 @@
         <v>1</v>
       </c>
       <c r="N19">
-        <v>0.1277565889922272</v>
+        <v>0.04395604395604396</v>
       </c>
       <c r="O19">
-        <v>0.345445251675922</v>
+        <v>0.2838441198097348</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -1374,7 +1374,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-0.3620604069403616</v>
+        <v>-0.1666666666666667</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1386,13 +1386,13 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>-0.1744749017817276</v>
+        <v>-0.1617550423176264</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20">
-        <v>0.4401255147930893</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1410,10 +1410,10 @@
         <v>1</v>
       </c>
       <c r="N20">
-        <v>-0.03891007767443947</v>
+        <v>-0.1318681318681319</v>
       </c>
       <c r="O20">
-        <v>0.08094357265170955</v>
+        <v>0.02833364993287087</v>
       </c>
       <c r="P20">
         <v>0</v>
@@ -1424,7 +1424,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.1388570472629527</v>
+        <v>0.25</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1436,13 +1436,13 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>1.956873432624048</v>
+        <v>1.731475523789778</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21">
-        <v>-1.242932775485466</v>
+        <v>-1.392857142857143</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1460,10 +1460,10 @@
         <v>2</v>
       </c>
       <c r="N21">
-        <v>0.002756588992227194</v>
+        <v>-0.08791208791208792</v>
       </c>
       <c r="O21">
-        <v>-0.1902878798244194</v>
+        <v>-0.2336778281160683</v>
       </c>
       <c r="P21">
         <v>0</v>
@@ -1474,7 +1474,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1.140691955669581</v>
+        <v>1.083333333333333</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1486,13 +1486,13 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>-0.3076841726820885</v>
+        <v>-0.2800819526993392</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>-0.4839064877127843</v>
+        <v>-0.5714285714285714</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1510,10 +1510,10 @@
         <v>2</v>
       </c>
       <c r="N22">
-        <v>-0.3305767443411061</v>
+        <v>-0.4395604395604396</v>
       </c>
       <c r="O22">
-        <v>-0.1105508556011127</v>
+        <v>-0.1566513056340883</v>
       </c>
       <c r="P22">
         <v>0</v>
@@ -1524,7 +1524,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.7399579923069298</v>
+        <v>0.75</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1536,13 +1536,13 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>0.05081677093356957</v>
+        <v>0.03836667133599051</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>-0.648912202445976</v>
+        <v>-0.75</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1560,10 +1560,10 @@
         <v>2</v>
       </c>
       <c r="N23">
-        <v>0.7527565889922272</v>
+        <v>0.7032967032967034</v>
       </c>
       <c r="O23">
-        <v>-0.15212315028164</v>
+        <v>-0.1968104327400777</v>
       </c>
       <c r="P23">
         <v>0</v>
@@ -1574,7 +1574,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.6397745014662669</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1586,13 +1586,13 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <v>0.005749405906995781</v>
+        <v>-0.001665692977662392</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="H24">
-        <v>0.506127800686366</v>
+        <v>0.5</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1610,10 +1610,10 @@
         <v>1</v>
       </c>
       <c r="N24">
-        <v>0.6694232556588938</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="O24">
-        <v>0.1302391680435261</v>
+        <v>0.07595353948476222</v>
       </c>
       <c r="P24">
         <v>0</v>
@@ -1624,7 +1624,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>-0.762794370303013</v>
+        <v>-0.5</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1636,13 +1636,13 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>1.494558904205149</v>
+        <v>1.320811540700304</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25">
-        <v>-0.8469190601258061</v>
+        <v>-0.9642857142857143</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -1660,10 +1660,10 @@
         <v>2</v>
       </c>
       <c r="N25">
-        <v>0.5860899223255606</v>
+        <v>0.5274725274725275</v>
       </c>
       <c r="O25">
-        <v>-0.2579435367411644</v>
+        <v>-0.2990336653735059</v>
       </c>
       <c r="P25">
         <v>0</v>
@@ -1674,7 +1674,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>-0.06150993441837302</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1686,13 +1686,13 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <v>0.9695576600684317</v>
+        <v>0.8544643056664952</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>-0.7809167742325294</v>
+        <v>-0.8928571428571429</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1710,10 +1710,10 @@
         <v>1</v>
       </c>
       <c r="N26">
-        <v>0.3777565889922272</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="O26">
-        <v>0.1454469590105555</v>
+        <v>0.09064437180805768</v>
       </c>
       <c r="P26">
         <v>0</v>
@@ -1724,7 +1724,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-0.06150993441837302</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1736,13 +1736,13 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <v>-0.7151478248478987</v>
+        <v>-0.6420230903375195</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
-        <v>0.1959170569879654</v>
+        <v>0.1642857142857141</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -1760,10 +1760,10 @@
         <v>1</v>
       </c>
       <c r="N27">
-        <v>0.6694232556588938</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="O27">
-        <v>-0.7590786526173396</v>
+        <v>-0.7831336884875253</v>
       </c>
       <c r="P27">
         <v>0</v>
@@ -1774,7 +1774,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>-0.4622438977810244</v>
+        <v>-0.25</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1786,13 +1786,13 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>0.6717957604088013</v>
+        <v>0.589968858930902</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0.605131229526281</v>
+        <v>0.6071428571428571</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1810,10 +1810,10 @@
         <v>1</v>
       </c>
       <c r="N28">
-        <v>-0.2472434110077728</v>
+        <v>-0.3516483516483517</v>
       </c>
       <c r="O28">
-        <v>0.7125805790733299</v>
+        <v>0.6384994110645057</v>
       </c>
       <c r="P28">
         <v>0</v>
@@ -1824,7 +1824,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.2390405381036155</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1836,13 +1836,13 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <v>-1.122611477013709</v>
+        <v>-1.0039642279757</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="H29">
-        <v>0.2751198000598976</v>
+        <v>0.25</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -1860,10 +1860,10 @@
         <v>1</v>
       </c>
       <c r="N29">
-        <v>0.4610899223255605</v>
+        <v>0.3956043956043956</v>
       </c>
       <c r="O29">
-        <v>0.104668546063565</v>
+        <v>0.05125214000311487</v>
       </c>
       <c r="P29">
         <v>0</v>
@@ -1874,7 +1874,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1.341058937350907</v>
+        <v>1.25</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1886,13 +1886,13 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <v>-1.240149068984616</v>
+        <v>-1.108370325371329</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30">
-        <v>0.9351426589926644</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -1910,10 +1910,10 @@
         <v>1</v>
       </c>
       <c r="N30">
-        <v>-0.2055767443411061</v>
+        <v>-0.3076923076923077</v>
       </c>
       <c r="O30">
-        <v>-0.2456608133128271</v>
+        <v>-0.2871684687285547</v>
       </c>
       <c r="P30">
         <v>0</v>
@@ -1924,7 +1924,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>-0.1616934252590359</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1936,13 +1936,13 @@
         <v>1</v>
       </c>
       <c r="F31">
-        <v>1.071423573109884</v>
+        <v>0.9449495900760402</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>-0.1868962011930392</v>
+        <v>-0.25</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -1960,10 +1960,10 @@
         <v>1</v>
       </c>
       <c r="N31">
-        <v>0.1277565889922272</v>
+        <v>0.04395604395604396</v>
       </c>
       <c r="O31">
-        <v>-0.1105508556011127</v>
+        <v>-0.1566513056340883</v>
       </c>
       <c r="P31">
         <v>1</v>
@@ -1974,7 +1974,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.5395910106256041</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1986,13 +1986,13 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <v>0.4132130580728063</v>
+        <v>0.3602754446605183</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>-1.011924774858998</v>
+        <v>-1.142857142857143</v>
       </c>
       <c r="I32">
         <v>1</v>
@@ -2010,10 +2010,10 @@
         <v>1</v>
       </c>
       <c r="N32">
-        <v>-0.1222434110077728</v>
+        <v>-0.2197802197802198</v>
       </c>
       <c r="O32">
-        <v>-0.8054020666899279</v>
+        <v>-0.8278824301199141</v>
       </c>
       <c r="P32">
         <v>1</v>
@@ -2024,7 +2024,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.2390405381036155</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2036,13 +2036,13 @@
         <v>1</v>
       </c>
       <c r="F33">
-        <v>0.6169448841557112</v>
+        <v>0.5412460134796082</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33">
-        <v>0.2421186571132592</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -2060,10 +2060,10 @@
         <v>2</v>
       </c>
       <c r="N33">
-        <v>0.002756588992227194</v>
+        <v>-0.08791208791208792</v>
       </c>
       <c r="O33">
-        <v>-0.1877565457220926</v>
+        <v>-0.2312325416880693</v>
       </c>
       <c r="P33">
         <v>0</v>
@@ -2074,7 +2074,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>-0.06150993441837302</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2086,13 +2086,13 @@
         <v>1</v>
       </c>
       <c r="F34">
-        <v>-0.856192935212987</v>
+        <v>-0.7673104072122744</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
-        <v>0.4731266577397276</v>
+        <v>0.4642857142857143</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -2110,10 +2110,10 @@
         <v>1</v>
       </c>
       <c r="N34">
-        <v>-1.080576744341106</v>
+        <v>-1.230769230769231</v>
       </c>
       <c r="O34">
-        <v>0.3144552249677737</v>
+        <v>0.2539075374980184</v>
       </c>
       <c r="P34">
         <v>1</v>
@@ -2124,7 +2124,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>-1.163528333665664</v>
+        <v>-0.8333333333333334</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2136,13 +2136,13 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>-0.1117881860639106</v>
+        <v>-0.106071790373291</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
-        <v>0.704134658366196</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -2160,10 +2160,10 @@
         <v>1</v>
       </c>
       <c r="N35">
-        <v>-0.7889100776744394</v>
+        <v>-0.9230769230769231</v>
       </c>
       <c r="O35">
-        <v>-0.3220273111498822</v>
+        <v>-0.3609390391732523</v>
       </c>
       <c r="P35">
         <v>0</v>
@@ -2174,7 +2174,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>-0.5624273886216873</v>
+        <v>-0.3333333333333333</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2186,13 +2186,13 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <v>0.1232869978779028</v>
+        <v>0.1027404044179668</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36">
-        <v>-0.05489162940648584</v>
+        <v>-0.1071428571428571</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -2210,10 +2210,10 @@
         <v>1</v>
       </c>
       <c r="N36">
-        <v>-0.2055767443411061</v>
+        <v>-0.3076923076923077</v>
       </c>
       <c r="O36">
-        <v>-0.1105508556011127</v>
+        <v>-0.1566513056340883</v>
       </c>
       <c r="P36">
         <v>0</v>
@@ -2224,7 +2224,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.03867355642228983</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2236,13 +2236,13 @@
         <v>1</v>
       </c>
       <c r="F37">
-        <v>-0.7778345405657157</v>
+        <v>-0.697706342281855</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
-        <v>0.5391289436330043</v>
+        <v>0.5357142857142857</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -2260,10 +2260,10 @@
         <v>1</v>
       </c>
       <c r="N37">
-        <v>1.21108992232556</v>
+        <v>1.186813186813187</v>
       </c>
       <c r="O37">
-        <v>-0.1105508556011127</v>
+        <v>-0.1566513056340883</v>
       </c>
       <c r="P37">
         <v>0</v>
@@ -2274,7 +2274,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>-0.8629778611436758</v>
+        <v>-0.5833333333333334</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2286,13 +2286,13 @@
         <v>1</v>
       </c>
       <c r="F38">
-        <v>-0.2438811114349323</v>
+        <v>-0.2234070751983714</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>0.6381323724729193</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -2310,10 +2310,10 @@
         <v>1</v>
       </c>
       <c r="N38">
-        <v>-0.5805767443411062</v>
+        <v>-0.7032967032967034</v>
       </c>
       <c r="O38">
-        <v>-0.1105508556011127</v>
+        <v>-0.1566513056340883</v>
       </c>
       <c r="P38">
         <v>1</v>
@@ -2324,7 +2324,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>-0.6626108794623501</v>
+        <v>-0.4166666666666667</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2336,13 +2336,13 @@
         <v>1</v>
       </c>
       <c r="F39">
-        <v>-1.686791918474062</v>
+        <v>-1.505113495474719</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>0.2091175141666209</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -2360,10 +2360,10 @@
         <v>2</v>
       </c>
       <c r="N39">
-        <v>0.4194232556588939</v>
+        <v>0.3516483516483517</v>
       </c>
       <c r="O39">
-        <v>0.4298889752457434</v>
+        <v>0.3654173467437762</v>
       </c>
       <c r="P39">
         <v>0</v>
@@ -2374,7 +2374,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>-1.764629278709641</v>
+        <v>-1.333333333333333</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2386,13 +2386,13 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0.1546303557368113</v>
+        <v>0.1305820303901345</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40">
-        <v>0.9351426589926644</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -2410,10 +2410,10 @@
         <v>2</v>
       </c>
       <c r="N40">
-        <v>0.04442325565889386</v>
+        <v>-0.04395604395604396</v>
       </c>
       <c r="O40">
-        <v>0.3894822589207442</v>
+        <v>0.3263841764725334</v>
       </c>
       <c r="P40">
         <v>0</v>
@@ -2424,7 +2424,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.1388570472629527</v>
+        <v>0.25</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2436,13 +2436,13 @@
         <v>1</v>
       </c>
       <c r="F41">
-        <v>1.502394743669875</v>
+        <v>1.327771947193346</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
-        <v>0.506127800686366</v>
+        <v>0.5</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -2460,10 +2460,10 @@
         <v>1</v>
       </c>
       <c r="N41">
-        <v>0.7527565889922272</v>
+        <v>0.7032967032967034</v>
       </c>
       <c r="O41">
-        <v>0.2368747499432945</v>
+        <v>0.1789642566088243</v>
       </c>
       <c r="P41">
         <v>1</v>
@@ -2474,7 +2474,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>-0.5624273886216873</v>
+        <v>-0.3333333333333333</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2486,13 +2486,13 @@
         <v>1</v>
       </c>
       <c r="F42">
-        <v>-0.5662668750180835</v>
+        <v>-0.5097753669697229</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>0.5721300865796426</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="I42">
         <v>0</v>
@@ -2510,10 +2510,10 @@
         <v>1</v>
       </c>
       <c r="N42">
-        <v>-0.1639100776744395</v>
+        <v>-0.2637362637362637</v>
       </c>
       <c r="O42">
-        <v>-0.5694148629239145</v>
+        <v>-0.5999171425586897</v>
       </c>
       <c r="P42">
         <v>0</v>
@@ -2524,7 +2524,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>-1.263711824506327</v>
+        <v>-0.9166666666666666</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2536,13 +2536,13 @@
         <v>1</v>
       </c>
       <c r="F43">
-        <v>0.4523922553964417</v>
+        <v>0.3950774771257278</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="H43">
-        <v>0.1431152282733442</v>
+        <v>0.1071428571428571</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -2560,10 +2560,10 @@
         <v>1</v>
       </c>
       <c r="N43">
-        <v>0.08608992232556052</v>
+        <v>0</v>
       </c>
       <c r="O43">
-        <v>-0.3336682169599063</v>
+        <v>-0.3721842355148578</v>
       </c>
       <c r="P43">
         <v>0</v>
@@ -2574,7 +2574,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>-0.06150993441837302</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2586,13 +2586,13 @@
         <v>1</v>
       </c>
       <c r="F44">
-        <v>-0.1744749017817276</v>
+        <v>-0.1617550423176264</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44">
-        <v>-0.1538950582464009</v>
+        <v>-0.2142857142857143</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -2610,10 +2610,10 @@
         <v>1</v>
       </c>
       <c r="N44">
-        <v>1.46108992232556</v>
+        <v>1.450549450549451</v>
       </c>
       <c r="O44">
-        <v>-1.101357212153682</v>
+        <v>-1.113777168326839</v>
       </c>
       <c r="P44">
         <v>0</v>
@@ -2624,7 +2624,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>-1.464078806187653</v>
+        <v>-1.083333333333333</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2636,13 +2636,13 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <v>0.500325504637158</v>
+        <v>0.4376555443193615</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
       <c r="H45">
-        <v>1.265154088459048</v>
+        <v>1.321428571428571</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -2660,10 +2660,10 @@
         <v>1</v>
       </c>
       <c r="N45">
-        <v>1.08608992232556</v>
+        <v>1.054945054945055</v>
       </c>
       <c r="O45">
-        <v>0.5467408305639825</v>
+        <v>0.4782970553660171</v>
       </c>
       <c r="P45">
         <v>0</v>
@@ -2674,7 +2674,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0.03867355642228983</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -2686,13 +2686,13 @@
         <v>1</v>
       </c>
       <c r="F46">
-        <v>-1.106939798084255</v>
+        <v>-0.990043414989616</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
-        <v>0.9351426589926644</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -2710,10 +2710,10 @@
         <v>1</v>
       </c>
       <c r="N46">
-        <v>0.1694232556588939</v>
+        <v>0.08791208791208792</v>
       </c>
       <c r="O46">
-        <v>0.1824586912435687</v>
+        <v>0.126397963727405</v>
       </c>
       <c r="P46">
         <v>0</v>
@@ -2724,7 +2724,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>-0.6626108794623501</v>
+        <v>-0.4166666666666667</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2736,13 +2736,13 @@
         <v>1</v>
       </c>
       <c r="F47">
-        <v>-0.1352957044580921</v>
+        <v>-0.1269530098524169</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47">
-        <v>0.04411179943342918</v>
+        <v>0</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -2760,10 +2760,10 @@
         <v>2</v>
       </c>
       <c r="N47">
-        <v>0.9610899223255606</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="O47">
-        <v>-0.7492524738746692</v>
+        <v>-0.7736415311715639</v>
       </c>
       <c r="P47">
         <v>0</v>
@@ -2774,7 +2774,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>-0.4622438977810244</v>
+        <v>-0.25</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2786,13 +2786,13 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>1.62776817510551</v>
+        <v>1.439138451082017</v>
       </c>
       <c r="G48">
         <v>1</v>
       </c>
       <c r="H48">
-        <v>0.1101140853267059</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="I48">
         <v>0</v>
@@ -2810,10 +2810,10 @@
         <v>2</v>
       </c>
       <c r="N48">
-        <v>1.544423255658894</v>
+        <v>1.538461538461539</v>
       </c>
       <c r="O48">
-        <v>0.623631556115371</v>
+        <v>0.5525740334452748</v>
       </c>
       <c r="P48">
         <v>0</v>
@@ -2824,7 +2824,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.4394075197849412</v>
+        <v>0.5</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2836,13 +2836,13 @@
         <v>1</v>
       </c>
       <c r="F49">
-        <v>-0.8875362930718954</v>
+        <v>-0.7951520331844421</v>
       </c>
       <c r="G49">
         <v>1</v>
       </c>
       <c r="H49">
-        <v>-0.747915631285891</v>
+        <v>-0.8571428571428571</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -2860,10 +2860,10 @@
         <v>1</v>
       </c>
       <c r="N49">
-        <v>0.5027565889922272</v>
+        <v>0.4395604395604396</v>
       </c>
       <c r="O49">
-        <v>-1.694165243663993</v>
+        <v>-1.686433868415737</v>
       </c>
       <c r="P49">
         <v>0</v>
@@ -2874,7 +2874,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>-0.5624273886216873</v>
+        <v>-0.3333333333333333</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -2886,13 +2886,13 @@
         <v>1</v>
       </c>
       <c r="F50">
-        <v>0.953885981138977</v>
+        <v>0.8405434926804111</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
       <c r="H50">
-        <v>0.4401255147930893</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="I50">
         <v>0</v>
@@ -2910,10 +2910,10 @@
         <v>1</v>
       </c>
       <c r="N50">
-        <v>0.9610899223255606</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="O50">
-        <v>-0.1105508556011127</v>
+        <v>-0.1566513056340883</v>
       </c>
       <c r="P50">
         <v>0</v>
@@ -2924,7 +2924,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.03867355642228983</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -2936,13 +2936,13 @@
         <v>1</v>
       </c>
       <c r="F51">
-        <v>0.7579899945207991</v>
+        <v>0.6665333303543628</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
       <c r="H51">
-        <v>-0.1868962011930392</v>
+        <v>-0.25</v>
       </c>
       <c r="I51">
         <v>0</v>
@@ -2960,10 +2960,10 @@
         <v>1</v>
       </c>
       <c r="N51">
-        <v>-0.3722434110077728</v>
+        <v>-0.4835164835164835</v>
       </c>
       <c r="O51">
-        <v>-0.1105508556011127</v>
+        <v>-0.1566513056340883</v>
       </c>
       <c r="P51">
         <v>1</v>
@@ -2974,7 +2974,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.03867355642228983</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2986,13 +2986,13 @@
         <v>1</v>
       </c>
       <c r="F52">
-        <v>1.235976201869154</v>
+        <v>1.091118126429921</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52">
-        <v>-0.648912202445976</v>
+        <v>-0.75</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -3010,10 +3010,10 @@
         <v>1</v>
       </c>
       <c r="N52">
-        <v>1.21108992232556</v>
+        <v>1.186813186813187</v>
       </c>
       <c r="O52">
-        <v>0.3758449921610583</v>
+        <v>0.3132104815059903</v>
       </c>
       <c r="P52">
         <v>0</v>
@@ -3024,7 +3024,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.1388570472629527</v>
+        <v>0.25</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -3036,13 +3036,13 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>-0.339027530540997</v>
+        <v>-0.3079235786715069</v>
       </c>
       <c r="G53">
         <v>1</v>
       </c>
       <c r="H53">
-        <v>-0.6819133453926144</v>
+        <v>-0.7857142857142857</v>
       </c>
       <c r="I53">
         <v>0</v>
@@ -3060,10 +3060,10 @@
         <v>1</v>
       </c>
       <c r="N53">
-        <v>0.2110899223255605</v>
+        <v>0.1318681318681319</v>
       </c>
       <c r="O53">
-        <v>-0.6942258729157171</v>
+        <v>-0.7204854502021818</v>
       </c>
       <c r="P53">
         <v>0</v>
@@ -3074,7 +3074,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>-1.36389531534699</v>
+        <v>-1</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -3086,13 +3086,13 @@
         <v>1</v>
       </c>
       <c r="F54">
-        <v>-0.009922273022458123</v>
+        <v>-0.01558650596374595</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
       <c r="H54">
-        <v>0.9021415160460261</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="I54">
         <v>0</v>
@@ -3110,10 +3110,10 @@
         <v>1</v>
       </c>
       <c r="N54">
-        <v>1.21108992232556</v>
+        <v>1.186813186813187</v>
       </c>
       <c r="O54">
-        <v>-0.08771536979068209</v>
+        <v>-0.1345920668012207</v>
       </c>
       <c r="P54">
         <v>0</v>
@@ -3124,7 +3124,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>-1.564262297028316</v>
+        <v>-1.166666666666667</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -3136,13 +3136,13 @@
         <v>1</v>
       </c>
       <c r="F55">
-        <v>-0.5427593566239023</v>
+        <v>-0.4888941474905972</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
       <c r="H55">
-        <v>0.704134658366196</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -3160,10 +3160,10 @@
         <v>1</v>
       </c>
       <c r="N55">
-        <v>1.46108992232556</v>
+        <v>1.450549450549451</v>
       </c>
       <c r="O55">
-        <v>-0.1105508556011127</v>
+        <v>-0.1566513056340883</v>
       </c>
       <c r="P55">
         <v>0</v>
@@ -3174,7 +3174,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>-1.664445787868979</v>
+        <v>-1.25</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -3186,13 +3186,13 @@
         <v>0</v>
       </c>
       <c r="F56">
-        <v>0.4288847370022602</v>
+        <v>0.3741962576466018</v>
       </c>
       <c r="G56">
         <v>0</v>
       </c>
       <c r="H56">
-        <v>0.7371358013128344</v>
+        <v>0.75</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -3210,10 +3210,10 @@
         <v>1</v>
       </c>
       <c r="N56">
-        <v>0.3777565889922272</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="O56">
-        <v>0.2768440673953058</v>
+        <v>0.2175748965128761</v>
       </c>
       <c r="P56">
         <v>0</v>
@@ -3224,7 +3224,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0.8401414831475926</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -3236,13 +3236,13 @@
         <v>1</v>
       </c>
       <c r="F57">
-        <v>-0.4957443198355395</v>
+        <v>-0.4471317085323456</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
       <c r="H57">
-        <v>0.1761163712199826</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="I57">
         <v>0</v>
@@ -3260,10 +3260,10 @@
         <v>1</v>
       </c>
       <c r="N57">
-        <v>0.3360899223255605</v>
+        <v>0.2637362637362637</v>
       </c>
       <c r="O57">
-        <v>0.0414478468245655</v>
+        <v>-0.009819497152813928</v>
       </c>
       <c r="P57">
         <v>0</v>
@@ -3274,7 +3274,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.8401414831475926</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -3286,13 +3286,13 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <v>-0.1431315439228191</v>
+        <v>-0.1339134163454587</v>
       </c>
       <c r="G58">
         <v>1</v>
       </c>
       <c r="H58">
-        <v>-0.8139179171791677</v>
+        <v>-0.9285714285714286</v>
       </c>
       <c r="I58">
         <v>0</v>
@@ -3310,10 +3310,10 @@
         <v>1</v>
       </c>
       <c r="N58">
-        <v>0.6277565889922272</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="O58">
-        <v>-0.5158807287362551</v>
+        <v>-0.548202794917487</v>
       </c>
       <c r="P58">
         <v>0</v>
@@ -3324,7 +3324,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0.9403249739882554</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -3336,13 +3336,13 @@
         <v>1</v>
       </c>
       <c r="F59">
-        <v>0.1546303557368113</v>
+        <v>0.1305820303901345</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59">
-        <v>0.2751198000598976</v>
+        <v>0.25</v>
       </c>
       <c r="I59">
         <v>0</v>
@@ -3360,10 +3360,10 @@
         <v>1</v>
       </c>
       <c r="N59">
-        <v>-1.205576744341106</v>
+        <v>-1.362637362637363</v>
       </c>
       <c r="O59">
-        <v>0.1105381661089648</v>
+        <v>0.05692223397503811</v>
       </c>
       <c r="P59">
         <v>1</v>
@@ -3374,7 +3374,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>1.641609409872895</v>
+        <v>1.5</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -3386,13 +3386,13 @@
         <v>1</v>
       </c>
       <c r="F60">
-        <v>-0.2293257780348176</v>
+        <v>-0.2104778877689202</v>
       </c>
       <c r="G60">
         <v>0</v>
       </c>
       <c r="H60">
-        <v>-0.3849030588728692</v>
+        <v>-0.4642857142857143</v>
       </c>
       <c r="I60">
         <v>0</v>
@@ -3410,10 +3410,10 @@
         <v>2</v>
       </c>
       <c r="N60">
-        <v>-0.4139100776744395</v>
+        <v>-0.5274725274725275</v>
       </c>
       <c r="O60">
-        <v>-0.4847015077258592</v>
+        <v>-0.5180834495879945</v>
       </c>
       <c r="P60">
         <v>0</v>
@@ -3424,7 +3424,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>1.040508464828918</v>
+        <v>1</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -3436,13 +3436,13 @@
         <v>1</v>
       </c>
       <c r="F61">
-        <v>-0.4748246010414983</v>
+        <v>-0.4285491753931567</v>
       </c>
       <c r="G61">
         <v>1</v>
       </c>
       <c r="H61">
-        <v>-0.7809167742325294</v>
+        <v>-0.8928571428571429</v>
       </c>
       <c r="I61">
         <v>1</v>
@@ -3460,10 +3460,10 @@
         <v>1</v>
       </c>
       <c r="N61">
-        <v>0.7527565889922272</v>
+        <v>0.7032967032967034</v>
       </c>
       <c r="O61">
-        <v>-1.616061812960211</v>
+        <v>-1.61098540868671</v>
       </c>
       <c r="P61">
         <v>1</v>
@@ -3474,7 +3474,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>-0.06150993441837302</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -3486,13 +3486,13 @@
         <v>0</v>
       </c>
       <c r="F62">
-        <v>0.1546303557368113</v>
+        <v>0.1305820303901345</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62">
-        <v>-0.3189007729795926</v>
+        <v>-0.3928571428571428</v>
       </c>
       <c r="I62">
         <v>1</v>
@@ -3510,10 +3510,10 @@
         <v>1</v>
       </c>
       <c r="N62">
-        <v>0.5860899223255606</v>
+        <v>0.5274725274725275</v>
       </c>
       <c r="O62">
-        <v>-1.709660492079481</v>
+        <v>-1.701402386642564</v>
       </c>
       <c r="P62">
         <v>1</v>
@@ -3524,7 +3524,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>-1.564262297028316</v>
+        <v>-1.166666666666667</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -3536,13 +3536,13 @@
         <v>1</v>
       </c>
       <c r="F63">
-        <v>1.447543867416786</v>
+        <v>1.279049101742053</v>
       </c>
       <c r="G63">
         <v>1</v>
       </c>
       <c r="H63">
-        <v>-0.08789277235312419</v>
+        <v>-0.1428571428571428</v>
       </c>
       <c r="I63">
         <v>0</v>
@@ -3560,10 +3560,10 @@
         <v>1</v>
       </c>
       <c r="N63">
-        <v>1.127756588992227</v>
+        <v>1.098901098901099</v>
       </c>
       <c r="O63">
-        <v>0.6930596754842121</v>
+        <v>0.619642081814736</v>
       </c>
       <c r="P63">
         <v>0</v>
@@ -3574,7 +3574,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.6397745014662669</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -3586,13 +3586,13 @@
         <v>1</v>
       </c>
       <c r="F64">
-        <v>0.1781378741309929</v>
+        <v>0.1514632498692605</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64">
-        <v>-0.747915631285891</v>
+        <v>-0.8571428571428571</v>
       </c>
       <c r="I64">
         <v>0</v>
@@ -3610,10 +3610,10 @@
         <v>2</v>
       </c>
       <c r="N64">
-        <v>-0.5805767443411062</v>
+        <v>-0.7032967032967034</v>
       </c>
       <c r="O64">
-        <v>0.03464193477565504</v>
+        <v>-0.01639405574152722</v>
       </c>
       <c r="P64">
         <v>1</v>
@@ -3624,7 +3624,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>1.040508464828918</v>
+        <v>1</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -3636,13 +3636,13 @@
         <v>1</v>
       </c>
       <c r="F65">
-        <v>-0.8953721325366224</v>
+        <v>-0.8021124396774839</v>
       </c>
       <c r="G65">
         <v>1</v>
       </c>
       <c r="H65">
-        <v>0.01111065648679084</v>
+        <v>-0.03571428571428571</v>
       </c>
       <c r="I65">
         <v>0</v>
@@ -3660,10 +3660,10 @@
         <v>2</v>
       </c>
       <c r="N65">
-        <v>-1.122243411007773</v>
+        <v>-1.274725274725275</v>
       </c>
       <c r="O65">
-        <v>-0.009218387317327478</v>
+        <v>-0.05876343331323894</v>
       </c>
       <c r="P65">
         <v>1</v>
@@ -3674,7 +3674,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>-1.664445787868979</v>
+        <v>-1.25</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -3686,13 +3686,13 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0.6874674393382552</v>
+        <v>0.6038896719169855</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>-0.2528984870863159</v>
+        <v>-0.3214285714285715</v>
       </c>
       <c r="I66">
         <v>0</v>
@@ -3710,10 +3710,10 @@
         <v>1</v>
       </c>
       <c r="N66">
-        <v>-0.1222434110077728</v>
+        <v>-0.2197802197802198</v>
       </c>
       <c r="O66">
-        <v>-0.2726828048551693</v>
+        <v>-0.3132719013474474</v>
       </c>
       <c r="P66">
         <v>0</v>
@@ -3724,7 +3724,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>-1.36389531534699</v>
+        <v>-1</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -3736,13 +3736,13 @@
         <v>1</v>
       </c>
       <c r="F67">
-        <v>1.753141606541144</v>
+        <v>1.550504954970688</v>
       </c>
       <c r="G67">
         <v>0</v>
       </c>
       <c r="H67">
-        <v>-0.2198973441396775</v>
+        <v>-0.2857142857142857</v>
       </c>
       <c r="I67">
         <v>0</v>
@@ -3760,10 +3760,10 @@
         <v>1</v>
       </c>
       <c r="N67">
-        <v>0.4194232556588939</v>
+        <v>0.3516483516483517</v>
       </c>
       <c r="O67">
-        <v>0.1596690598223153</v>
+        <v>0.104383020554844</v>
       </c>
       <c r="P67">
         <v>0</v>
@@ -3774,7 +3774,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0.9403249739882554</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -3786,13 +3786,13 @@
         <v>1</v>
       </c>
       <c r="F68">
-        <v>0.121254904093188</v>
+        <v>0.1009353395187599</v>
       </c>
       <c r="G68">
         <v>0</v>
       </c>
       <c r="H68">
-        <v>-1.671947633791764</v>
+        <v>-1.857142857142857</v>
       </c>
       <c r="I68">
         <v>0</v>
@@ -3810,10 +3810,10 @@
         <v>1</v>
       </c>
       <c r="N68">
-        <v>-1.430576744341106</v>
+        <v>-1.6</v>
       </c>
       <c r="O68">
-        <v>-0.3578707781920467</v>
+        <v>-0.3955640787561617</v>
       </c>
       <c r="P68">
         <v>0</v>
@@ -3824,7 +3824,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0.1388570472629527</v>
+        <v>0.25</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -3836,13 +3836,13 @@
         <v>1</v>
       </c>
       <c r="F69">
-        <v>-0.03851251975862625</v>
+        <v>-0.04098260295065961</v>
       </c>
       <c r="G69">
         <v>0</v>
       </c>
       <c r="H69">
-        <v>-0.5169076306594226</v>
+        <v>-0.6071428571428571</v>
       </c>
       <c r="I69">
         <v>1</v>
@@ -3860,10 +3860,10 @@
         <v>1</v>
       </c>
       <c r="N69">
-        <v>-1.16391007767444</v>
+        <v>-1.318681318681319</v>
       </c>
       <c r="O69">
-        <v>-1.452332504600204</v>
+        <v>-1.452821752917062</v>
       </c>
       <c r="P69">
         <v>1</v>
@@ -3874,7 +3874,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>-0.2618769160996987</v>
+        <v>-0.08333333333333333</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -3886,13 +3886,13 @@
         <v>0</v>
       </c>
       <c r="F70">
-        <v>0.1389586768073567</v>
+        <v>0.1166612174040504</v>
       </c>
       <c r="G70">
         <v>0</v>
       </c>
       <c r="H70">
-        <v>0.2421186571132592</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="I70">
         <v>0</v>
@@ -3910,10 +3910,10 @@
         <v>1</v>
       </c>
       <c r="N70">
-        <v>-0.6222434110077728</v>
+        <v>-0.7472527472527473</v>
       </c>
       <c r="O70">
-        <v>2.281559871098086</v>
+        <v>2.154144368825311</v>
       </c>
       <c r="P70">
         <v>0</v>
@@ -3924,7 +3924,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>-0.06150993441837302</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -3936,13 +3936,13 @@
         <v>1</v>
       </c>
       <c r="F71">
-        <v>0.3897055396786248</v>
+        <v>0.3393942251813923</v>
       </c>
       <c r="G71">
         <v>0</v>
       </c>
       <c r="H71">
-        <v>-0.2528984870863159</v>
+        <v>-0.3214285714285715</v>
       </c>
       <c r="I71">
         <v>0</v>
@@ -3960,10 +3960,10 @@
         <v>1</v>
       </c>
       <c r="N71">
-        <v>-1.497243411007773</v>
+        <v>-1.67032967032967</v>
       </c>
       <c r="O71">
-        <v>-0.6068731492359802</v>
+        <v>-0.6361021088382492</v>
       </c>
       <c r="P71">
         <v>1</v>
@@ -3974,7 +3974,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0.3392240289442784</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -3986,13 +3986,13 @@
         <v>0</v>
       </c>
       <c r="F72">
-        <v>0.8676917470269793</v>
+        <v>0.7639790212569502</v>
       </c>
       <c r="G72">
         <v>1</v>
       </c>
       <c r="H72">
-        <v>0.3081209430065359</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="I72">
         <v>0</v>
@@ -4010,10 +4010,10 @@
         <v>1</v>
       </c>
       <c r="N72">
-        <v>0.7944232556588938</v>
+        <v>0.7472527472527473</v>
       </c>
       <c r="O72">
-        <v>-0.9491643862255443</v>
+        <v>-0.9667578351859467</v>
       </c>
       <c r="P72">
         <v>0</v>
@@ -4024,7 +4024,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.4394075197849412</v>
+        <v>0.5</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -4036,13 +4036,13 @@
         <v>1</v>
       </c>
       <c r="F73">
-        <v>-0.4565651225119041</v>
+        <v>-0.4123296760671361</v>
       </c>
       <c r="G73">
         <v>1</v>
       </c>
       <c r="H73">
-        <v>0.1101140853267059</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="I73">
         <v>0</v>
@@ -4060,10 +4060,10 @@
         <v>1</v>
       </c>
       <c r="N73">
-        <v>1.252756588992227</v>
+        <v>1.230769230769231</v>
       </c>
       <c r="O73">
-        <v>0.1210662147618261</v>
+        <v>0.06709240252785413</v>
       </c>
       <c r="P73">
         <v>0</v>
@@ -4074,7 +4074,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0.03867355642228983</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -4086,13 +4086,13 @@
         <v>1</v>
       </c>
       <c r="F74">
-        <v>1.831500001188414</v>
+        <v>1.620109019901107</v>
       </c>
       <c r="G74">
         <v>0</v>
       </c>
       <c r="H74">
-        <v>0.04411179943342918</v>
+        <v>0</v>
       </c>
       <c r="I74">
         <v>0</v>
@@ -4110,10 +4110,10 @@
         <v>2</v>
       </c>
       <c r="N74">
-        <v>-1.205576744341106</v>
+        <v>-1.362637362637363</v>
       </c>
       <c r="O74">
-        <v>1.510768636939454</v>
+        <v>1.409554651499504</v>
       </c>
       <c r="P74">
         <v>0</v>
@@ -4124,7 +4124,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0.8401414831475926</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -4136,13 +4136,13 @@
         <v>1</v>
       </c>
       <c r="F75">
-        <v>0.6561240814793466</v>
+        <v>0.5760480459448177</v>
       </c>
       <c r="G75">
         <v>1</v>
       </c>
       <c r="H75">
-        <v>0.605131229526281</v>
+        <v>0.6071428571428571</v>
       </c>
       <c r="I75">
         <v>1</v>
@@ -4160,10 +4160,10 @@
         <v>1</v>
       </c>
       <c r="N75">
-        <v>-0.1639100776744395</v>
+        <v>-0.2637362637362637</v>
       </c>
       <c r="O75">
-        <v>-1.167933133344961</v>
+        <v>-1.17808997332991</v>
       </c>
       <c r="P75">
         <v>1</v>
@@ -4174,7 +4174,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>-0.6626108794623501</v>
+        <v>-0.4166666666666667</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -4186,13 +4186,13 @@
         <v>1</v>
       </c>
       <c r="F76">
-        <v>2.254635332283679</v>
+        <v>1.995970970525371</v>
       </c>
       <c r="G76">
         <v>0</v>
       </c>
       <c r="H76">
-        <v>1.760171232658623</v>
+        <v>1.857142857142857</v>
       </c>
       <c r="I76">
         <v>1</v>
@@ -4210,10 +4210,10 @@
         <v>1</v>
       </c>
       <c r="N76">
-        <v>0.6277565889922272</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="O76">
-        <v>0.862240839923228</v>
+        <v>0.7830722686460676</v>
       </c>
       <c r="P76">
         <v>1</v>
@@ -4224,7 +4224,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0.3392240289442784</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -4236,13 +4236,13 @@
         <v>1</v>
       </c>
       <c r="F77">
-        <v>-1.342014982026068</v>
+        <v>-1.198855609780874</v>
       </c>
       <c r="G77">
         <v>0</v>
       </c>
       <c r="H77">
-        <v>0.07711294238006752</v>
+        <v>0.03571428571428571</v>
       </c>
       <c r="I77">
         <v>0</v>
@@ -4260,10 +4260,10 @@
         <v>1</v>
       </c>
       <c r="N77">
-        <v>-0.1222434110077728</v>
+        <v>-0.2197802197802198</v>
       </c>
       <c r="O77">
-        <v>-0.6509906864479689</v>
+        <v>-0.6787199580119528</v>
       </c>
       <c r="P77">
         <v>0</v>
@@ -4274,7 +4274,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0.1388570472629527</v>
+        <v>0.25</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -4286,13 +4286,13 @@
         <v>0</v>
       </c>
       <c r="F78">
-        <v>-0.05693730981082122</v>
+        <v>-0.05734894492199787</v>
       </c>
       <c r="G78">
         <v>0</v>
       </c>
       <c r="H78">
-        <v>0.4731266577397276</v>
+        <v>0.4642857142857143</v>
       </c>
       <c r="I78">
         <v>0</v>
@@ -4310,10 +4310,10 @@
         <v>1</v>
       </c>
       <c r="N78">
-        <v>-0.5389100776744394</v>
+        <v>-0.6593406593406593</v>
       </c>
       <c r="O78">
-        <v>-0.2420091928341314</v>
+        <v>-0.283640977834109</v>
       </c>
       <c r="P78">
         <v>0</v>
@@ -4324,7 +4324,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0.4394075197849412</v>
+        <v>0.5</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -4336,13 +4336,13 @@
         <v>1</v>
       </c>
       <c r="F79">
-        <v>0.2486604293135369</v>
+        <v>0.2141069083066378</v>
       </c>
       <c r="G79">
         <v>1</v>
       </c>
       <c r="H79">
-        <v>-0.4839064877127843</v>
+        <v>-0.5714285714285714</v>
       </c>
       <c r="I79">
         <v>0</v>
@@ -4360,10 +4360,10 @@
         <v>2</v>
       </c>
       <c r="N79">
-        <v>0.08608992232556052</v>
+        <v>0</v>
       </c>
       <c r="O79">
-        <v>-0.02211524691708202</v>
+        <v>-0.07122188979043799</v>
       </c>
       <c r="P79">
         <v>0</v>
@@ -4374,7 +4374,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0.2390405381036155</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -4386,13 +4386,13 @@
         <v>1</v>
       </c>
       <c r="F80">
-        <v>0.6247807236204381</v>
+        <v>0.5482064199726501</v>
       </c>
       <c r="G80">
         <v>0</v>
       </c>
       <c r="H80">
-        <v>0.4071243718464509</v>
+        <v>0.3928571428571428</v>
       </c>
       <c r="I80">
         <v>0</v>
@@ -4410,10 +4410,10 @@
         <v>1</v>
       </c>
       <c r="N80">
-        <v>-0.1222434110077728</v>
+        <v>-0.2197802197802198</v>
       </c>
       <c r="O80">
-        <v>0.06316194717109155</v>
+        <v>0.01115647548736869</v>
       </c>
       <c r="P80">
         <v>0</v>
@@ -4424,7 +4424,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>-0.1616934252590359</v>
+        <v>0</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -4436,13 +4436,13 @@
         <v>1</v>
       </c>
       <c r="F81">
-        <v>1.565081459387692</v>
+        <v>1.383455199137682</v>
       </c>
       <c r="G81">
         <v>0</v>
       </c>
       <c r="H81">
-        <v>0.1431152282733442</v>
+        <v>0.1071428571428571</v>
       </c>
       <c r="I81">
         <v>0</v>
@@ -4460,10 +4460,10 @@
         <v>1</v>
       </c>
       <c r="N81">
-        <v>0.7527565889922272</v>
+        <v>0.7032967032967034</v>
       </c>
       <c r="O81">
-        <v>-0.2396824965999194</v>
+        <v>-0.2813933730164102</v>
       </c>
       <c r="P81">
         <v>0</v>
@@ -4474,7 +4474,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>-1.664445787868979</v>
+        <v>-1.25</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -4486,13 +4486,13 @@
         <v>1</v>
       </c>
       <c r="F82">
-        <v>-0.2528332964289992</v>
+        <v>-0.2313591072480461</v>
       </c>
       <c r="G82">
         <v>1</v>
       </c>
       <c r="H82">
-        <v>1.331156374352324</v>
+        <v>1.392857142857143</v>
       </c>
       <c r="I82">
         <v>0</v>
@@ -4510,10 +4510,10 @@
         <v>1</v>
       </c>
       <c r="N82">
-        <v>0.4610899223255605</v>
+        <v>0.3956043956043956</v>
       </c>
       <c r="O82">
-        <v>-0.9276958798415588</v>
+        <v>-0.946019108029419</v>
       </c>
       <c r="P82">
         <v>0</v>
@@ -4524,7 +4524,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>0.03867355642228983</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -4536,13 +4536,13 @@
         <v>1</v>
       </c>
       <c r="F83">
-        <v>0.9773934995331586</v>
+        <v>0.861424712159537</v>
       </c>
       <c r="G83">
         <v>1</v>
       </c>
       <c r="H83">
-        <v>-0.450905344766146</v>
+        <v>-0.5357142857142857</v>
       </c>
       <c r="I83">
         <v>0</v>
@@ -4560,10 +4560,10 @@
         <v>1</v>
       </c>
       <c r="N83">
-        <v>0.3777565889922272</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="O83">
-        <v>0.4392879288256884</v>
+        <v>0.3744968015677388</v>
       </c>
       <c r="P83">
         <v>0</v>
@@ -4574,7 +4574,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>-0.1616934252590359</v>
+        <v>0</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -4586,13 +4586,13 @@
         <v>1</v>
       </c>
       <c r="F84">
-        <v>0.2251529109193553</v>
+        <v>0.1932256888275118</v>
       </c>
       <c r="G84">
         <v>0</v>
       </c>
       <c r="H84">
-        <v>-0.648912202445976</v>
+        <v>-0.75</v>
       </c>
       <c r="I84">
         <v>1</v>
@@ -4610,10 +4610,10 @@
         <v>2</v>
       </c>
       <c r="N84">
-        <v>-0.2055767443411061</v>
+        <v>-0.3076923076923077</v>
       </c>
       <c r="O84">
-        <v>1.398953499522865</v>
+        <v>1.301540447559257</v>
       </c>
       <c r="P84">
         <v>0</v>
@@ -4624,7 +4624,7 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>-2.06517975123163</v>
+        <v>-1.583333333333333</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -4636,13 +4636,13 @@
         <v>1</v>
       </c>
       <c r="F85">
-        <v>-0.652461109130082</v>
+        <v>-0.5863398383931844</v>
       </c>
       <c r="G85">
         <v>1</v>
       </c>
       <c r="H85">
-        <v>0.4071243718464509</v>
+        <v>0.3928571428571428</v>
       </c>
       <c r="I85">
         <v>1</v>
@@ -4660,10 +4660,10 @@
         <v>1</v>
       </c>
       <c r="N85">
-        <v>1.252756588992227</v>
+        <v>1.230769230769231</v>
       </c>
       <c r="O85">
-        <v>-0.3257702572657897</v>
+        <v>-0.3645547512712908</v>
       </c>
       <c r="P85">
         <v>0</v>
@@ -4674,7 +4674,7 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>-0.2618769160996987</v>
+        <v>-0.08333333333333333</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -4686,13 +4686,13 @@
         <v>1</v>
       </c>
       <c r="F86">
-        <v>0.3270188239608077</v>
+        <v>0.2837109732370568</v>
       </c>
       <c r="G86">
         <v>5</v>
       </c>
       <c r="H86">
-        <v>0.6381323724729193</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="I86">
         <v>0</v>
@@ -4710,10 +4710,10 @@
         <v>2</v>
       </c>
       <c r="N86">
-        <v>0.9610899223255606</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="O86">
-        <v>0.2333654003923411</v>
+        <v>0.1755742004245528</v>
       </c>
       <c r="P86">
         <v>0</v>
@@ -4724,7 +4724,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>1.641609409872895</v>
+        <v>1.5</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -4736,13 +4736,13 @@
         <v>1</v>
       </c>
       <c r="F87">
-        <v>-1.271492426843524</v>
+        <v>-1.136211951343497</v>
       </c>
       <c r="G87">
         <v>1</v>
       </c>
       <c r="H87">
-        <v>-1.077927060752274</v>
+        <v>-1.214285714285714</v>
       </c>
       <c r="I87">
         <v>0</v>
@@ -4760,10 +4760,10 @@
         <v>1</v>
       </c>
       <c r="N87">
-        <v>-0.2472434110077728</v>
+        <v>-0.3516483516483517</v>
       </c>
       <c r="O87">
-        <v>0.3016490153837771</v>
+        <v>0.2415366495693674</v>
       </c>
       <c r="P87">
         <v>1</v>
@@ -4774,7 +4774,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0.4394075197849412</v>
+        <v>0.5</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -4786,13 +4786,13 @@
         <v>1</v>
       </c>
       <c r="F88">
-        <v>-0.002086433557731171</v>
+        <v>-0.008626099470704173</v>
       </c>
       <c r="G88">
         <v>0</v>
       </c>
       <c r="H88">
-        <v>-0.1208939152997625</v>
+        <v>-0.1785714285714286</v>
       </c>
       <c r="I88">
         <v>1</v>
@@ -4810,10 +4810,10 @@
         <v>2</v>
       </c>
       <c r="N88">
-        <v>0.4610899223255605</v>
+        <v>0.3956043956043956</v>
       </c>
       <c r="O88">
-        <v>-0.388491340036639</v>
+        <v>-0.4251437554284189</v>
       </c>
       <c r="P88">
         <v>1</v>
@@ -4824,7 +4824,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>0.6397745014662669</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -4836,13 +4836,13 @@
         <v>1</v>
       </c>
       <c r="F89">
-        <v>-0.009922273022458123</v>
+        <v>-0.01558650596374595</v>
       </c>
       <c r="G89">
         <v>0</v>
       </c>
       <c r="H89">
-        <v>-0.5499087736060609</v>
+        <v>-0.6428571428571429</v>
       </c>
       <c r="I89">
         <v>0</v>
@@ -4860,10 +4860,10 @@
         <v>1</v>
       </c>
       <c r="N89">
-        <v>-0.03891007767443947</v>
+        <v>-0.1318681318681319</v>
       </c>
       <c r="O89">
-        <v>-1.3179164351526</v>
+        <v>-1.322974890733573</v>
       </c>
       <c r="P89">
         <v>1</v>
@@ -4874,7 +4874,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>0.4394075197849412</v>
+        <v>0.5</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -4886,13 +4886,13 @@
         <v>1</v>
       </c>
       <c r="F90">
-        <v>0.4758997737906233</v>
+        <v>0.4159586966048537</v>
       </c>
       <c r="G90">
         <v>0</v>
       </c>
       <c r="H90">
-        <v>-0.2198973441396775</v>
+        <v>-0.2857142857142857</v>
       </c>
       <c r="I90">
         <v>0</v>
@@ -4910,10 +4910,10 @@
         <v>2</v>
       </c>
       <c r="N90">
-        <v>0.5860899223255606</v>
+        <v>0.5274725274725275</v>
       </c>
       <c r="O90">
-        <v>0.4453301132699392</v>
+        <v>0.3803335939545723</v>
       </c>
       <c r="P90">
         <v>0</v>
@@ -4924,7 +4924,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>-1.36389531534699</v>
+        <v>-1</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -4936,13 +4936,13 @@
         <v>1</v>
       </c>
       <c r="F91">
-        <v>-0.009922273022458123</v>
+        <v>-0.01558650596374595</v>
       </c>
       <c r="G91">
         <v>0</v>
       </c>
       <c r="H91">
-        <v>0.3378219716585106</v>
+        <v>0.3178571428571431</v>
       </c>
       <c r="I91">
         <v>0</v>
@@ -4960,10 +4960,10 @@
         <v>1</v>
       </c>
       <c r="N91">
-        <v>-0.03891007767443947</v>
+        <v>-0.1318681318681319</v>
       </c>
       <c r="O91">
-        <v>-0.3421679259640515</v>
+        <v>-0.3803950137960307</v>
       </c>
       <c r="P91">
         <v>0</v>
@@ -4974,7 +4974,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>-0.1616934252590359</v>
+        <v>0</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -4986,13 +4986,13 @@
         <v>1</v>
       </c>
       <c r="F92">
-        <v>-0.8170137378893515</v>
+        <v>-0.7325083747470649</v>
       </c>
       <c r="G92">
         <v>0</v>
       </c>
       <c r="H92">
-        <v>-0.4839064877127843</v>
+        <v>-0.5714285714285714</v>
       </c>
       <c r="I92">
         <v>0</v>
@@ -5010,10 +5010,10 @@
         <v>1</v>
       </c>
       <c r="N92">
-        <v>0.2527565889922272</v>
+        <v>0.1758241758241758</v>
       </c>
       <c r="O92">
-        <v>0.6691676789794656</v>
+        <v>0.5965622462698533</v>
       </c>
       <c r="P92">
         <v>0</v>
@@ -5024,7 +5024,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>1.240875446510244</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -5036,13 +5036,13 @@
         <v>1</v>
       </c>
       <c r="F93">
-        <v>-0.1352957044580921</v>
+        <v>-0.1269530098524169</v>
       </c>
       <c r="G93">
         <v>0</v>
       </c>
       <c r="H93">
-        <v>0.1431152282733442</v>
+        <v>0.1071428571428571</v>
       </c>
       <c r="I93">
         <v>0</v>
@@ -5060,10 +5060,10 @@
         <v>1</v>
       </c>
       <c r="N93">
-        <v>-1.247243411007773</v>
+        <v>-1.406593406593407</v>
       </c>
       <c r="O93">
-        <v>0.1723534802501742</v>
+        <v>0.1166362593077868</v>
       </c>
       <c r="P93">
         <v>1</v>
@@ -5074,7 +5074,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>-0.3620604069403616</v>
+        <v>-0.1666666666666667</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -5086,13 +5086,13 @@
         <v>1</v>
       </c>
       <c r="F94">
-        <v>0.9303784627447962</v>
+        <v>0.8196622732012857</v>
       </c>
       <c r="G94">
         <v>0</v>
       </c>
       <c r="H94">
-        <v>0.605131229526281</v>
+        <v>0.6071428571428571</v>
       </c>
       <c r="I94">
         <v>0</v>
@@ -5110,10 +5110,10 @@
         <v>1</v>
       </c>
       <c r="N94">
-        <v>-0.6222434110077728</v>
+        <v>-0.7472527472527473</v>
       </c>
       <c r="O94">
-        <v>-0.3578707781920467</v>
+        <v>-0.3955640787561617</v>
       </c>
       <c r="P94">
         <v>0</v>
@@ -5124,7 +5124,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.6397745014662669</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -5136,13 +5136,13 @@
         <v>0</v>
       </c>
       <c r="F95">
-        <v>-0.05693730981082122</v>
+        <v>-0.05734894492199787</v>
       </c>
       <c r="G95">
         <v>1</v>
       </c>
       <c r="H95">
-        <v>-0.450905344766146</v>
+        <v>-0.5357142857142857</v>
       </c>
       <c r="I95">
         <v>1</v>
@@ -5160,10 +5160,10 @@
         <v>1</v>
       </c>
       <c r="N95">
-        <v>0.5860899223255606</v>
+        <v>0.5274725274725275</v>
       </c>
       <c r="O95">
-        <v>-2.695898154517153</v>
+        <v>-2.654114858901169</v>
       </c>
       <c r="P95">
         <v>1</v>
@@ -5174,7 +5174,7 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>-0.762794370303013</v>
+        <v>-0.5</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -5186,13 +5186,13 @@
         <v>1</v>
       </c>
       <c r="F96">
-        <v>-0.1666390623170006</v>
+        <v>-0.1547946358245847</v>
       </c>
       <c r="G96">
         <v>1</v>
       </c>
       <c r="H96">
-        <v>0.3411220859531743</v>
+        <v>0.3214285714285715</v>
       </c>
       <c r="I96">
         <v>0</v>
@@ -5210,10 +5210,10 @@
         <v>1</v>
       </c>
       <c r="N96">
-        <v>-1.66391007767444</v>
+        <v>-1.846153846153846</v>
       </c>
       <c r="O96">
-        <v>-0.4396909029589728</v>
+        <v>-0.4746028909168482</v>
       </c>
       <c r="P96">
         <v>0</v>
@@ -5224,7 +5224,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>-0.8629778611436758</v>
+        <v>-0.5833333333333334</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -5236,13 +5236,13 @@
         <v>1</v>
       </c>
       <c r="F97">
-        <v>-1.114775637548982</v>
+        <v>-0.9970038214826581</v>
       </c>
       <c r="G97">
         <v>1</v>
       </c>
       <c r="H97">
-        <v>-0.08789277235312419</v>
+        <v>-0.1428571428571428</v>
       </c>
       <c r="I97">
         <v>0</v>
@@ -5260,10 +5260,10 @@
         <v>1</v>
       </c>
       <c r="N97">
-        <v>-0.08057674434110614</v>
+        <v>-0.1758241758241758</v>
       </c>
       <c r="O97">
-        <v>0.3526832851247642</v>
+        <v>0.2908361106897959</v>
       </c>
       <c r="P97">
         <v>0</v>
@@ -5274,7 +5274,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>-0.5624273886216873</v>
+        <v>-0.3333333333333333</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -5286,13 +5286,13 @@
         <v>1</v>
       </c>
       <c r="F98">
-        <v>-0.3860425673293602</v>
+        <v>-0.3496860176297589</v>
       </c>
       <c r="G98">
         <v>0</v>
       </c>
       <c r="H98">
-        <v>0.4731266577397276</v>
+        <v>0.4642857142857143</v>
       </c>
       <c r="I98">
         <v>0</v>
@@ -5310,10 +5310,10 @@
         <v>1</v>
       </c>
       <c r="N98">
-        <v>1.21108992232556</v>
+        <v>1.186813186813187</v>
       </c>
       <c r="O98">
-        <v>-0.4498967959003016</v>
+        <v>-0.4844618548015848</v>
       </c>
       <c r="P98">
         <v>0</v>
@@ -5324,7 +5324,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>1.140691955669581</v>
+        <v>1.083333333333333</v>
       </c>
       <c r="C99">
         <v>1</v>
@@ -5336,13 +5336,13 @@
         <v>1</v>
       </c>
       <c r="F99">
-        <v>-1.067760600760619</v>
+        <v>-0.9552413825244065</v>
       </c>
       <c r="G99">
         <v>0</v>
       </c>
       <c r="H99">
-        <v>-0.1538950582464009</v>
+        <v>-0.2142857142857143</v>
       </c>
       <c r="I99">
         <v>0</v>
@@ -5360,10 +5360,10 @@
         <v>1</v>
       </c>
       <c r="N99">
-        <v>-0.7472434110077728</v>
+        <v>-0.8791208791208791</v>
       </c>
       <c r="O99">
-        <v>1.227037725744855</v>
+        <v>1.135468609001125</v>
       </c>
       <c r="P99">
         <v>0</v>
@@ -5374,7 +5374,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>1.541425919032233</v>
+        <v>1.416666666666667</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -5386,13 +5386,13 @@
         <v>1</v>
       </c>
       <c r="F100">
-        <v>-1.075596440225346</v>
+        <v>-0.9622017890174486</v>
       </c>
       <c r="G100">
         <v>0</v>
       </c>
       <c r="H100">
-        <v>-1.110928203698913</v>
+        <v>-1.25</v>
       </c>
       <c r="I100">
         <v>0</v>
@@ -5410,10 +5410,10 @@
         <v>1</v>
       </c>
       <c r="N100">
-        <v>-1.622243411007773</v>
+        <v>-1.802197802197802</v>
       </c>
       <c r="O100">
-        <v>0.3316271878190415</v>
+        <v>0.2704957735841638</v>
       </c>
       <c r="P100">
         <v>1</v>
@@ -5424,7 +5424,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>0.03867355642228983</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -5436,13 +5436,13 @@
         <v>0</v>
       </c>
       <c r="F101">
-        <v>0.1856597816841608</v>
+        <v>0.1581447974441959</v>
       </c>
       <c r="G101">
         <v>0</v>
       </c>
       <c r="H101">
-        <v>0.01971386332968701</v>
+        <v>-0.0264037782647978</v>
       </c>
       <c r="I101">
         <v>0</v>
@@ -5460,10 +5460,10 @@
         <v>1</v>
       </c>
       <c r="N101">
-        <v>0.09741644772481332</v>
+        <v>0.0119488619596513</v>
       </c>
       <c r="O101">
-        <v>-1.347150468555783</v>
+        <v>-1.351215171244456</v>
       </c>
       <c r="P101">
         <v>1</v>
@@ -5474,7 +5474,7 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>1.841976391554221</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -5486,13 +5486,13 @@
         <v>1</v>
       </c>
       <c r="F102">
-        <v>-0.7543270221715345</v>
+        <v>-0.6768251228027293</v>
       </c>
       <c r="G102">
         <v>0</v>
       </c>
       <c r="H102">
-        <v>-0.9459224889657211</v>
+        <v>-1.071428571428571</v>
       </c>
       <c r="I102">
         <v>0</v>
@@ -5510,10 +5510,10 @@
         <v>1</v>
       </c>
       <c r="N102">
-        <v>0.6694232556588938</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="O102">
-        <v>0.3901507523893569</v>
+        <v>0.3270299458336391</v>
       </c>
       <c r="P102">
         <v>0</v>
@@ -5524,7 +5524,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>-0.8629778611436758</v>
+        <v>-0.5833333333333334</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -5536,13 +5536,13 @@
         <v>0</v>
       </c>
       <c r="F103">
-        <v>1.259483720263335</v>
+        <v>1.111999345909047</v>
       </c>
       <c r="G103">
         <v>0</v>
       </c>
       <c r="H103">
-        <v>0.8361392301527494</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="I103">
         <v>0</v>
@@ -5560,10 +5560,10 @@
         <v>0</v>
       </c>
       <c r="N103">
-        <v>0.2110899223255605</v>
+        <v>0.1318681318681319</v>
       </c>
       <c r="O103">
-        <v>0.6868193866319532</v>
+        <v>0.6136139191857114</v>
       </c>
       <c r="P103">
         <v>1</v>
@@ -5574,7 +5574,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>-0.2618769160996987</v>
+        <v>-0.08333333333333333</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -5586,13 +5586,13 @@
         <v>1</v>
       </c>
       <c r="F104">
-        <v>2.38784460318404</v>
+        <v>2.114297880907084</v>
       </c>
       <c r="G104">
         <v>1</v>
       </c>
       <c r="H104">
-        <v>-0.2858996300329542</v>
+        <v>-0.3571428571428572</v>
       </c>
       <c r="I104">
         <v>0</v>
@@ -5610,10 +5610,10 @@
         <v>1</v>
       </c>
       <c r="N104">
-        <v>1.08608992232556</v>
+        <v>1.054945054945055</v>
       </c>
       <c r="O104">
-        <v>0.4089010206497483</v>
+        <v>0.3451428359718197</v>
       </c>
       <c r="P104">
         <v>0</v>
@@ -5624,7 +5624,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>-0.1616934252590359</v>
+        <v>0</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -5636,13 +5636,13 @@
         <v>1</v>
       </c>
       <c r="F105">
-        <v>0.2443019339767648</v>
+        <v>0.2102353512924184</v>
       </c>
       <c r="G105">
         <v>0</v>
       </c>
       <c r="H105">
-        <v>0.1101140853267059</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="I105">
         <v>0</v>
@@ -5660,10 +5660,10 @@
         <v>1</v>
       </c>
       <c r="N105">
-        <v>0.5444232556588938</v>
+        <v>0.4835164835164835</v>
       </c>
       <c r="O105">
-        <v>1.510768636939454</v>
+        <v>1.409554651499504</v>
       </c>
       <c r="P105">
         <v>0</v>
@@ -5674,7 +5674,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>-1.36389531534699</v>
+        <v>-1</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -5686,13 +5686,13 @@
         <v>2</v>
       </c>
       <c r="F106">
-        <v>-0.9423871693249851</v>
+        <v>-0.8438748786357355</v>
       </c>
       <c r="G106">
         <v>0</v>
       </c>
       <c r="H106">
-        <v>0.605131229526281</v>
+        <v>0.6071428571428571</v>
       </c>
       <c r="I106">
         <v>0</v>
@@ -5710,10 +5710,10 @@
         <v>1</v>
       </c>
       <c r="N106">
-        <v>0.08608992232556052</v>
+        <v>0</v>
       </c>
       <c r="O106">
-        <v>-0.1105508556011127</v>
+        <v>-0.1566513056340883</v>
       </c>
       <c r="P106">
         <v>0</v>

</xml_diff>